<commit_message>
Changes from PR review
</commit_message>
<xml_diff>
--- a/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
+++ b/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
@@ -552,20 +552,20 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,11 +839,11 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C17" s="10"/>

</xml_diff>

<commit_message>
Last visit - add extra field data:
Who the lead visitor was and their relation to the prisoner.
If the visit was attended or not
If the visit was canceled what the reason was
</commit_message>
<xml_diff>
--- a/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
+++ b/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t xml:space="preserve">NOMIS Database Tables - Level Hierarchy</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t xml:space="preserve">OFFENDER_IEP_LEVELS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFFENDER_VISIT_VISITORS</t>
   </si>
   <si>
     <t xml:space="preserve">IMPRISONMENT_STATUSES</t>
@@ -551,8 +554,8 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -565,7 +568,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,7 +806,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="n">
         <v>9</v>
       </c>
@@ -817,7 +820,9 @@
       <c r="E15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
     </row>
@@ -826,14 +831,14 @@
         <v>10</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -844,12 +849,12 @@
         <v>11</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -860,12 +865,12 @@
         <v>12</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -876,12 +881,12 @@
         <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
@@ -892,12 +897,12 @@
         <v>14</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -908,12 +913,12 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -924,12 +929,12 @@
         <v>16</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -940,12 +945,12 @@
         <v>17</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -956,12 +961,12 @@
         <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
@@ -972,12 +977,12 @@
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -988,12 +993,12 @@
         <v>20</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -1004,12 +1009,12 @@
         <v>21</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -1020,12 +1025,12 @@
         <v>22</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -1036,12 +1041,12 @@
         <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -1052,12 +1057,12 @@
         <v>24</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -1068,12 +1073,12 @@
         <v>25</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -1084,7 +1089,7 @@
         <v>26</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -1098,7 +1103,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -1112,7 +1117,7 @@
         <v>28</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -1126,7 +1131,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -1140,7 +1145,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -1154,7 +1159,7 @@
         <v>31</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>

</xml_diff>

<commit_message>
NN-1026 Only one main activity - get pay rates
</commit_message>
<xml_diff>
--- a/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
+++ b/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t xml:space="preserve">NOMIS Database Tables - Level Hierarchy</t>
   </si>
@@ -151,6 +151,9 @@
     <t xml:space="preserve">OIC_HEARINGS</t>
   </si>
   <si>
+    <t xml:space="preserve">OFFENDER_PRG_PRF_PAY_BANDS</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONTACT_PERSON_TYPES</t>
   </si>
   <si>
@@ -308,6 +311,9 @@
   </si>
   <si>
     <t xml:space="preserve">STATUTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COURSE_ACTIVITY_PAY_RATES</t>
   </si>
   <si>
     <t xml:space="preserve">SYSTEM_PROFILES</t>
@@ -564,14 +570,14 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28"/>
@@ -735,7 +741,7 @@
       </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="n">
         <v>5</v>
       </c>
@@ -752,7 +758,9 @@
       <c r="F11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="10"/>
+      <c r="G11" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -760,17 +768,17 @@
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -780,17 +788,17 @@
         <v>7</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -800,17 +808,17 @@
         <v>8</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -820,17 +828,17 @@
         <v>9</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -840,14 +848,14 @@
         <v>10</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -858,14 +866,14 @@
         <v>11</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -876,14 +884,14 @@
         <v>12</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -894,14 +902,14 @@
         <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
@@ -912,12 +920,12 @@
         <v>14</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -928,12 +936,12 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -944,12 +952,12 @@
         <v>16</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -960,12 +968,12 @@
         <v>17</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -976,12 +984,12 @@
         <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
@@ -992,12 +1000,12 @@
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -1008,12 +1016,12 @@
         <v>20</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -1024,12 +1032,12 @@
         <v>21</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -1040,12 +1048,12 @@
         <v>22</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -1056,12 +1064,12 @@
         <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -1072,12 +1080,12 @@
         <v>24</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -1088,37 +1096,39 @@
         <v>25</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="n">
         <v>26</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+      <c r="E32" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="n">
         <v>27</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -1132,7 +1142,7 @@
         <v>28</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -1146,7 +1156,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -1160,7 +1170,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -1174,7 +1184,7 @@
         <v>31</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>

</xml_diff>

<commit_message>
NN-1124 Create a new endpoint to expose court events
</commit_message>
<xml_diff>
--- a/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
+++ b/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t xml:space="preserve">NOMIS Database Tables - Level Hierarchy</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t xml:space="preserve">OFFENDER_IMAGES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COURT_EVENTS</t>
   </si>
   <si>
     <t xml:space="preserve">INTERNAL_SCHEDULE_REASONS</t>
@@ -569,8 +572,8 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -843,7 +846,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="n">
         <v>10</v>
       </c>
@@ -857,7 +860,9 @@
       <c r="E16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="10"/>
+      <c r="F16" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
     </row>
@@ -866,14 +871,14 @@
         <v>11</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -884,14 +889,14 @@
         <v>12</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -902,14 +907,14 @@
         <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
@@ -920,12 +925,12 @@
         <v>14</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -936,12 +941,12 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -952,12 +957,12 @@
         <v>16</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -968,12 +973,12 @@
         <v>17</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -984,12 +989,12 @@
         <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
@@ -1000,12 +1005,12 @@
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -1016,12 +1021,12 @@
         <v>20</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -1032,12 +1037,12 @@
         <v>21</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -1048,12 +1053,12 @@
         <v>22</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -1064,12 +1069,12 @@
         <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -1080,12 +1085,12 @@
         <v>24</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -1096,12 +1101,12 @@
         <v>25</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -1112,12 +1117,12 @@
         <v>26</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
@@ -1128,7 +1133,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -1142,7 +1147,7 @@
         <v>28</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -1156,7 +1161,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -1170,7 +1175,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -1184,7 +1189,7 @@
         <v>31</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>

</xml_diff>

<commit_message>
NN-1168 Establishment roll - API endpoint rollcounts
</commit_message>
<xml_diff>
--- a/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
+++ b/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t xml:space="preserve">NOMIS Database Tables - Level Hierarchy</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t xml:space="preserve">SYSTEM_PROFILES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIVING_UNITS_MV</t>
   </si>
   <si>
     <t xml:space="preserve">TAG_ERROR_LOGS</t>
@@ -572,8 +575,8 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1137,17 +1140,19 @@
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
     </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="n">
         <v>28</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -1161,7 +1166,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -1175,7 +1180,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -1189,7 +1194,7 @@
         <v>31</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>

</xml_diff>

<commit_message>
NN-779 [Personal tab] Show Ethnicity Code, nationality and spoken language
</commit_message>
<xml_diff>
--- a/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
+++ b/mobile-web/src/main/resources/db/migration/nomis/data/nomis_data_hierarchy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve">NOMIS Database Tables - Level Hierarchy</t>
   </si>
@@ -328,7 +328,13 @@
     <t xml:space="preserve">TAG_ERROR_LOGS</t>
   </si>
   <si>
+    <t xml:space="preserve">OFFENDER_HEALTH_PROBLEMS</t>
+  </si>
+  <si>
     <t xml:space="preserve">TAG_IMAGES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFFENDER_LANGUAGES</t>
   </si>
   <si>
     <t xml:space="preserve">TRUST_AUDITS_TMP</t>
@@ -575,8 +581,8 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1156,21 +1162,25 @@
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
+      <c r="E34" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="n">
         <v>29</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
+      <c r="E35" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
@@ -1180,7 +1190,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -1194,7 +1204,7 @@
         <v>31</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>

</xml_diff>